<commit_message>
Opcao de densidade ser dada via polinomio.
</commit_message>
<xml_diff>
--- a/doc/air_prop.xlsx
+++ b/doc/air_prop.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="10200" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="10200" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Entrada" sheetId="1" r:id="rId1"/>
@@ -1683,47 +1683,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout>
         <c:manualLayout>
+          <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38961891260339643"/>
-          <c:y val="1.9028746606704072E-2"/>
+          <c:x val="3.6825551379137289E-2"/>
+          <c:y val="0.14084580856467721"/>
+          <c:w val="0.92357322951690735"/>
+          <c:h val="0.81969994574823557"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1775,7 +1747,8 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="power"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -1947,6 +1920,169 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-53BF-4551-A252-D4038A098863}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Polinomio</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>density!$B$39:$B$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>123.14999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>173.14999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>223.14999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>273.14999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>293.14999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>313.14999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>333.15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>353.15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>373.15</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>393.15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>413.15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>433.15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>453.15</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>473.15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>523.15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>573.15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>623.15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>673.15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>density!$C$39:$C$56</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>2.6886516886314791</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0307922940496921</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5875327499213467</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2905452597157456</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2007428797977155</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1234326181679846</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0563927055822973</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99772815246361368</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9458452182658359</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89942588083758856</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.85740230578595344</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.81893131584023671</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.7833688602157256</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.75024448397743448</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.67627972515528612</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.61366272016940115</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.56247638769467656</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.52260370093814501</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C992-4C1D-8D96-D0711AC442B5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9431,15 +9567,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>85724</xdr:colOff>
+      <xdr:colOff>161924</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9933,7 +10069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="D2" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A37"/>
     </sheetView>
   </sheetViews>
@@ -10828,8 +10964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A35:F57"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39:C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10844,15 +10980,23 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
-        <v>314.55916966863202</v>
-      </c>
-      <c r="B36">
-        <v>-0.98115089269056399</v>
-      </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
+        <v>-6.6486031886552598E-14</v>
+      </c>
+      <c r="B36" s="10">
+        <v>1.8919937609291901E-10</v>
+      </c>
+      <c r="C36" s="10">
+        <v>-2.14542924896456E-7</v>
+      </c>
+      <c r="D36" s="10">
+        <v>1.2345238441682701E-4</v>
+      </c>
+      <c r="E36" s="10">
+        <v>-3.7837036735780802E-2</v>
+      </c>
+      <c r="F36" s="10">
+        <v>5.8350781029802796</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
@@ -10868,12 +11012,8 @@
         <v>123.14999999999998</v>
       </c>
       <c r="C39" s="10">
-        <f>$A$36*POWER(B39,$B$36)</f>
-        <v>2.7968601829408017</v>
-      </c>
-      <c r="D39" s="10">
-        <f>$A$36*POWER(A39,5)+$B$36*POWER(C39,4)+$C$36*POWER(C39,3)+$D$36*POWER(C39,2)+$E$36*POWER(C39,1)+$F$36</f>
-        <v>-23886836946771.781</v>
+        <f>$A$36*POWER(B39,5)+$B$36*POWER(B39,4)+$C$36*POWER(B39,3)+$D$36*POWER(B39,2)+$E$36*POWER(B39,1)+$F$36</f>
+        <v>2.6886516886314791</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10885,12 +11025,8 @@
         <v>173.14999999999998</v>
       </c>
       <c r="C40" s="10">
-        <f t="shared" ref="C40:C56" si="1">$A$36*POWER(B40,$B$36)</f>
-        <v>2.0020370931817246</v>
-      </c>
-      <c r="D40" s="10">
-        <f t="shared" ref="D40:D56" si="2">$A$36*POWER(A40,5)+$B$36*POWER(C40,4)+$C$36*POWER(C40,3)+$D$36*POWER(C40,2)+$E$36*POWER(C40,1)+$F$36</f>
-        <v>-3145591696702.083</v>
+        <f t="shared" ref="C40:C56" si="1">$A$36*POWER(B40,5)+$B$36*POWER(B40,4)+$C$36*POWER(B40,3)+$D$36*POWER(B40,2)+$E$36*POWER(B40,1)+$F$36</f>
+        <v>2.0307922940496921</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10903,11 +11039,7 @@
       </c>
       <c r="C41" s="10">
         <f t="shared" si="1"/>
-        <v>1.5608976020042145</v>
-      </c>
-      <c r="D41" s="10">
-        <f t="shared" si="2"/>
-        <v>-98299740527.271667</v>
+        <v>1.5875327499213467</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10920,11 +11052,7 @@
       </c>
       <c r="C42" s="10">
         <f t="shared" si="1"/>
-        <v>1.2800446908885788</v>
-      </c>
-      <c r="D42" s="10">
-        <f t="shared" si="2"/>
-        <v>-2.6341247200280797</v>
+        <v>1.2905452597157456</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10937,11 +11065,7 @@
       </c>
       <c r="C43" s="10">
         <f t="shared" si="1"/>
-        <v>1.1943040182064302</v>
-      </c>
-      <c r="D43" s="10">
-        <f t="shared" si="2"/>
-        <v>1006589340.9434624</v>
+        <v>1.2007428797977155</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10954,11 +11078,7 @@
       </c>
       <c r="C44" s="10">
         <f t="shared" si="1"/>
-        <v>1.1194189094720561</v>
-      </c>
-      <c r="D44" s="10">
-        <f t="shared" si="2"/>
-        <v>32210858972.527264</v>
+        <v>1.1234326181679846</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10971,11 +11091,7 @@
       </c>
       <c r="C45" s="10">
         <f t="shared" si="1"/>
-        <v>1.0534454235443167</v>
-      </c>
-      <c r="D45" s="10">
-        <f t="shared" si="2"/>
-        <v>244601210333.11993</v>
+        <v>1.0563927055822973</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10988,11 +11104,7 @@
       </c>
       <c r="C46" s="10">
         <f t="shared" si="1"/>
-        <v>0.99487815680676406</v>
-      </c>
-      <c r="D46" s="10">
-        <f t="shared" si="2"/>
-        <v>1030747487169.2123</v>
+        <v>0.99772815246361368</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -11005,11 +11117,7 @@
       </c>
       <c r="C47" s="10">
         <f t="shared" si="1"/>
-        <v>0.94253310023635262</v>
-      </c>
-      <c r="D47" s="10">
-        <f t="shared" si="2"/>
-        <v>3145591696685.5459</v>
+        <v>0.9458452182658359</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -11022,14 +11130,10 @@
       </c>
       <c r="C48" s="10">
         <f t="shared" si="1"/>
-        <v>0.89546615763738924</v>
-      </c>
-      <c r="D48" s="10">
-        <f t="shared" si="2"/>
-        <v>7827238730697.873</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.89942588083758856</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>140</v>
       </c>
@@ -11039,14 +11143,10 @@
       </c>
       <c r="C49" s="10">
         <f t="shared" si="1"/>
-        <v>0.85291526750532931</v>
-      </c>
-      <c r="D49" s="10">
-        <f t="shared" si="2"/>
-        <v>16917747086785.715</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.85740230578595344</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>160</v>
       </c>
@@ -11056,14 +11156,10 @@
       </c>
       <c r="C50" s="10">
         <f t="shared" si="1"/>
-        <v>0.81425851648956737</v>
-      </c>
-      <c r="D50" s="10">
-        <f t="shared" si="2"/>
-        <v>32983919589445.121</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.81893131584023671</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>180</v>
       </c>
@@ -11073,14 +11169,10 @@
       </c>
       <c r="C51" s="10">
         <f t="shared" si="1"/>
-        <v>0.77898331498449602</v>
-      </c>
-      <c r="D51" s="10">
-        <f t="shared" si="2"/>
-        <v>59438094111241.406</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.7833688602157256</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>200</v>
       </c>
@@ -11090,14 +11182,10 @@
       </c>
       <c r="C52" s="10">
         <f t="shared" si="1"/>
-        <v>0.74666336911006459</v>
-      </c>
-      <c r="D52" s="10">
-        <f t="shared" si="2"/>
-        <v>100658934293961.94</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.75024448397743448</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>250</v>
       </c>
@@ -11107,14 +11195,10 @@
       </c>
       <c r="C53" s="10">
         <f t="shared" si="1"/>
-        <v>0.67658100006067423</v>
-      </c>
-      <c r="D53" s="10">
-        <f t="shared" si="2"/>
-        <v>307186689129523.25</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.67627972515528612</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>300</v>
       </c>
@@ -11124,14 +11208,10 @@
       </c>
       <c r="C54" s="10">
         <f t="shared" si="1"/>
-        <v>0.61862141229750611</v>
-      </c>
-      <c r="D54" s="10">
-        <f t="shared" si="2"/>
-        <v>764378782294775.75</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.61366272016940115</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>350</v>
       </c>
@@ -11141,14 +11221,10 @@
       </c>
       <c r="C55" s="10">
         <f t="shared" si="1"/>
-        <v>0.56988250704358701</v>
-      </c>
-      <c r="D55" s="10">
-        <f t="shared" si="2"/>
-        <v>1652123738943968.3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.56247638769467656</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>400</v>
       </c>
@@ -11158,14 +11234,10 @@
       </c>
       <c r="C56" s="10">
         <f t="shared" si="1"/>
-        <v>0.52832101188228975</v>
-      </c>
-      <c r="D56" s="10">
-        <f t="shared" si="2"/>
-        <v>3221085897406792</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+        <v>0.52260370093814501</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -12491,7 +12563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A35:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C13" workbookViewId="0">
       <selection activeCell="N60" sqref="N60"/>
     </sheetView>
   </sheetViews>

</xml_diff>